<commit_message>
feat: write test scripts for payment and shipping page
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ORDER_TEST_DATA.xlsx
+++ b/src/test/resources/testdata/ORDER_TEST_DATA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9432" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9432" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT_DETAIL_PAGE" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
   <si>
     <t>TEST_CASE</t>
   </si>
@@ -79,6 +79,9 @@
     <t>Huyện Kỳ Anh</t>
   </si>
   <si>
+    <t>Negative</t>
+  </si>
+  <si>
     <t>NAME</t>
   </si>
   <si>
@@ -100,6 +103,12 @@
     <t>COMMENT</t>
   </si>
   <si>
+    <t>EDIT_DISTRICT</t>
+  </si>
+  <si>
+    <t>EDIT_COMMUNE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nguyen Nam </t>
   </si>
   <si>
@@ -118,9 +127,6 @@
     <t>test thoi nha may chi</t>
   </si>
   <si>
-    <t>Negative</t>
-  </si>
-  <si>
     <t>0356356534</t>
   </si>
   <si>
@@ -128,6 +134,33 @@
   </si>
   <si>
     <t>bank</t>
+  </si>
+  <si>
+    <t>verifyOrderFailsWhenNameIsAllDigits</t>
+  </si>
+  <si>
+    <t>4234123421342</t>
+  </si>
+  <si>
+    <t>verifyOrderFailsWhenPhoneIsEmpty</t>
+  </si>
+  <si>
+    <t>verifyOrderFailsWhenPhoneIsInvalid</t>
+  </si>
+  <si>
+    <t>abc12‍3-+=!hehehe</t>
+  </si>
+  <si>
+    <t>verifyOrderSucceedsWhenEmailIsEmpty</t>
+  </si>
+  <si>
+    <t>verifyOrderFailsWhenEmailIsInvalid</t>
+  </si>
+  <si>
+    <t>verifyOrderSucceedsWhenDistrictAndCommuneAreEdited</t>
+  </si>
+  <si>
+    <t>Bến Nghé</t>
   </si>
 </sst>
 </file>
@@ -137,9 +170,9 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -160,7 +193,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -168,14 +201,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,8 +215,75 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,6 +297,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -211,23 +305,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -236,7 +313,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,50 +334,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -311,91 +344,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,91 +506,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,15 +549,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -553,17 +577,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -592,13 +621,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -607,152 +640,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -762,10 +795,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="48" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -1173,52 +1203,52 @@
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="5"/>
+      <c r="A5" s="4"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="5"/>
+      <c r="A6" s="4"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="5"/>
+      <c r="A8" s="4"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="5"/>
+      <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="5"/>
+      <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="5"/>
+      <c r="A11" s="4"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="5"/>
+      <c r="A12" s="4"/>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="5"/>
+      <c r="A13" s="4"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="5"/>
+      <c r="A14" s="4"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="5"/>
+      <c r="A15" s="4"/>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="5"/>
+      <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="5"/>
+      <c r="A17" s="4"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="5"/>
+      <c r="A18" s="4"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="5"/>
+      <c r="A19" s="4"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="5"/>
+      <c r="A20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1229,13 +1259,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="4"/>
   <cols>
     <col min="3" max="6" width="18" customWidth="1"/>
   </cols>
@@ -1306,6 +1336,14 @@
       </c>
       <c r="E4" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1317,18 +1355,19 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
+    <col min="1" max="1" width="44.2222222222222" customWidth="1"/>
     <col min="3" max="12" width="14.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="48" customHeight="1" spans="1:11">
+    <row r="1" s="1" customFormat="1" ht="48" customHeight="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1336,13 +1375,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>12</v>
@@ -1351,16 +1390,22 @@
         <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="48" customHeight="1" spans="1:11">
@@ -1371,13 +1416,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
@@ -1389,13 +1434,13 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="1" ht="48" customHeight="1" spans="1:11">
@@ -1403,16 +1448,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -1424,22 +1469,235 @@
         <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" ht="48" customHeight="1"/>
     <row r="5" ht="48" customHeight="1"/>
-    <row r="6" ht="48" customHeight="1"/>
+    <row r="6" customFormat="1" ht="48" customHeight="1" spans="1:11">
+      <c r="A6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" customFormat="1" spans="1:11">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" customFormat="1" spans="1:11">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" customFormat="1" spans="1:11">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" customFormat="1" spans="1:13">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11">
+        <v>13</v>
+      </c>
+      <c r="I11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="hellobitches@example.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="hellobitches@example.com" tooltip="mailto:hellobitches@example.com"/>
     <hyperlink ref="E3" r:id="rId1" display="invalid_email.com"/>
+    <hyperlink ref="E6" r:id="rId1" display="hellobitches@example.com" tooltip="mailto:hellobitches@example.com"/>
+    <hyperlink ref="E7" r:id="rId1" display="hellobitches@example.com" tooltip="mailto:hellobitches@example.com"/>
+    <hyperlink ref="E10" r:id="rId1" display="invalid_email.com" tooltip="mailto:hellobitches@example.com"/>
+    <hyperlink ref="E11" r:id="rId1" display="hellobitches@example.com" tooltip="mailto:hellobitches@example.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feat: complete testing shipping and payment, setup singleton driver
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ORDER_TEST_DATA.xlsx
+++ b/src/test/resources/testdata/ORDER_TEST_DATA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9432" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9432" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT_DETAIL_PAGE" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="50">
   <si>
     <t>TEST_CASE</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>Kỳ Xuân</t>
+  </si>
+  <si>
+    <t>verifyOrderFailsWhenDistrictCommuneAndAddressAreEmpty</t>
+  </si>
+  <si>
+    <t>verifyOrderFailsWhenTermsAndConditionsNotChecked</t>
   </si>
 </sst>
 </file>
@@ -169,9 +175,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -207,6 +213,81 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -216,25 +297,17 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -246,90 +319,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -344,13 +350,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -362,25 +482,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,139 +524,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -535,6 +541,41 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -549,6 +590,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -572,36 +622,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -620,162 +641,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1261,7 +1267,7 @@
   <sheetPr/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1355,10 +1361,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1525,7 +1531,6 @@
       <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="D7"/>
       <c r="E7" s="3" t="s">
         <v>32</v>
       </c>
@@ -1614,7 +1619,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" customFormat="1" spans="1:11">
+    <row r="10" customFormat="1" ht="15" customHeight="1" spans="1:11">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1688,6 +1693,76 @@
       </c>
       <c r="M11" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="12" customFormat="1" spans="1:13">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" customFormat="1" ht="48" customHeight="1" spans="1:11">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13">
+        <v>13</v>
+      </c>
+      <c r="I13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1698,6 +1773,8 @@
     <hyperlink ref="E7" r:id="rId1" display="hellobitches@example.com" tooltip="mailto:hellobitches@example.com"/>
     <hyperlink ref="E10" r:id="rId1" display="invalid_email.com" tooltip="mailto:hellobitches@example.com"/>
     <hyperlink ref="E11" r:id="rId1" display="hellobitches@example.com" tooltip="mailto:hellobitches@example.com"/>
+    <hyperlink ref="E12" r:id="rId1" display="hellobitches@example.com" tooltip="mailto:hellobitches@example.com"/>
+    <hyperlink ref="E13" r:id="rId1" display="hellobitches@example.com" tooltip="mailto:hellobitches@example.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feat: test payment in view cart page
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ORDER_TEST_DATA.xlsx
+++ b/src/test/resources/testdata/ORDER_TEST_DATA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9432" activeTab="1"/>
+    <workbookView windowWidth="11472" windowHeight="9264"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT_DETAIL_PAGE" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="82">
   <si>
     <t>TEST_CASE</t>
   </si>
@@ -28,6 +28,12 @@
     <t>PRODUCT_URL</t>
   </si>
   <si>
+    <t>PRODUCT_NAME</t>
+  </si>
+  <si>
+    <t>PRODUCT_PRICE</t>
+  </si>
+  <si>
     <t>SIZE</t>
   </si>
   <si>
@@ -46,16 +52,34 @@
     <t>https://theblues.com.vn/san-pham/ao-so-mi-nam-hoa-tiet-hk1-ms22n023ubr4/</t>
   </si>
   <si>
+    <t>Áo Sơ Mi Nam Họa Tiết HK1-MS22N023UBR4</t>
+  </si>
+  <si>
+    <t>399000</t>
+  </si>
+  <si>
     <t>L</t>
   </si>
   <si>
     <t>https://theblues.com.vn/san-pham/thun-croptop-in-hinh-tvm-t2m-19-478/</t>
   </si>
   <si>
+    <t>Thun Croptop In Hình TVM-T2M/19-478</t>
+  </si>
+  <si>
+    <t>125000</t>
+  </si>
+  <si>
     <t>M</t>
   </si>
   <si>
-    <t>https://theblues.com.vn/san-pham/ao-nam-the-thao-co-tron-tvm-t1s-22-711/\</t>
+    <t>https://theblues.com.vn/san-pham/ao-nam-the-thao-co-tron-tvm-t1s-22-711/</t>
+  </si>
+  <si>
+    <t>Áo Nam Thể Thao Cổ Trơn TVM-T1S/22-711</t>
+  </si>
+  <si>
+    <t>179000</t>
   </si>
   <si>
     <t>TC_AC_2</t>
@@ -92,6 +116,9 @@
   </si>
   <si>
     <t>DISTRICT</t>
+  </si>
+  <si>
+    <t>SHIPPING_RATE</t>
   </si>
   <si>
     <t>TC_VC_1</t>
@@ -243,11 +270,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -282,8 +309,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -297,29 +345,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -333,7 +407,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -348,67 +436,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -419,13 +446,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,7 +566,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,157 +620,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,17 +640,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -660,6 +705,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -669,44 +723,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -715,142 +742,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -876,7 +903,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="48">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
@@ -1201,20 +1228,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="17.4444444444444" customWidth="1"/>
     <col min="3" max="3" width="68.1111111111111" customWidth="1"/>
-    <col min="4" max="20" width="17.4444444444444" customWidth="1"/>
+    <col min="4" max="4" width="32.4444444444444" customWidth="1"/>
+    <col min="5" max="22" width="17.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="30" customHeight="1" spans="1:6">
+    <row r="1" s="1" customFormat="1" ht="30" customHeight="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1233,133 +1261,157 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" ht="30" customHeight="1" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" ht="30" customHeight="1" spans="1:8">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1" spans="1:8">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" ht="30" customHeight="1" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3">
+    </row>
+    <row r="4" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="30" customHeight="1" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" ht="30" customHeight="1" spans="1:9">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" customFormat="1" ht="30" customHeight="1" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" customFormat="1" ht="30" customHeight="1" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F8" t="s">
         <v>17</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="1" ht="30" customHeight="1" spans="1:7">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" customFormat="1" ht="30" customHeight="1" spans="1:6">
-      <c r="A8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -1408,7 +1460,7 @@
     <hyperlink ref="C6" r:id="rId2" display="https://theblues.com.vn/san-pham/thun-croptop-in-hinh-tvm-t2m-19-478/"/>
     <hyperlink ref="C7" r:id="rId2" display="https://theblues.com.vn/san-pham/thun-croptop-in-hinh-tvm-t2m-19-478/"/>
     <hyperlink ref="C3" r:id="rId2" display="https://theblues.com.vn/san-pham/thun-croptop-in-hinh-tvm-t2m-19-478/"/>
-    <hyperlink ref="C4" r:id="rId3" display="https://theblues.com.vn/san-pham/ao-nam-the-thao-co-tron-tvm-t1s-22-711/\" tooltip="https://theblues.com.vn/san-pham/ao-nam-the-thao-co-tron-tvm-t1s-22-711/\"/>
+    <hyperlink ref="C4" r:id="rId3" display="https://theblues.com.vn/san-pham/ao-nam-the-thao-co-tron-tvm-t1s-22-711/" tooltip="https://theblues.com.vn/san-pham/ao-nam-the-thao-co-tron-tvm-t1s-22-711/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1418,163 +1470,181 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
     <col min="2" max="2" width="25.4444444444444" customWidth="1"/>
     <col min="4" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:6">
+    <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" customFormat="1" spans="1:6">
       <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:6">
       <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1604,75 +1674,75 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" ht="48" customHeight="1" spans="3:12">
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I2">
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="L2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="1" ht="48" customHeight="1" spans="1:12">
@@ -1680,312 +1750,312 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I3">
         <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="K3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="L3" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" ht="48" customHeight="1"/>
     <row r="5" ht="48" customHeight="1"/>
     <row r="6" customFormat="1" ht="48" customHeight="1" spans="2:12">
       <c r="B6" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I6">
         <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="K6" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="L6" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="2:12">
       <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I7">
         <v>13</v>
       </c>
       <c r="J7" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="K7" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="L7" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="2:12">
       <c r="B8" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I8">
         <v>13</v>
       </c>
       <c r="J8" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="K8" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="L8" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="2:12">
       <c r="B9" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I9">
         <v>13</v>
       </c>
       <c r="J9" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="K9" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="L9" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="1" ht="15" customHeight="1" spans="2:12">
       <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I10">
         <v>13</v>
       </c>
       <c r="J10" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="K10" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="L10" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" customFormat="1" spans="2:14">
       <c r="B11" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I11">
         <v>13</v>
       </c>
       <c r="J11" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="K11" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="L11" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="M11" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="N11" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" customFormat="1" spans="2:14">
       <c r="B12" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="K12" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="L12" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="M12" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="N12" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" customFormat="1" ht="48" customHeight="1" spans="2:12">
       <c r="B13" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H13" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I13">
         <v>13</v>
       </c>
       <c r="J13" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="K13" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="L13" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>